<commit_message>
sofia | test | bug fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/test/SSS_Sofia_test4.xlsx
+++ b/assets/fleet/9245263_sofia/test/SSS_Sofia_test4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0AA7A8-B31D-4DF4-BF65-537A59F24C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4CCD52-1671-4FFC-862A-6C4FC33C59D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="59" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="214">
   <si>
     <t>Форпик</t>
   </si>
@@ -1259,7 +1259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1622C7A3-F812-43D4-BDBF-973F36BAE217}">
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
@@ -3560,7 +3560,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3638,8 +3638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C7A2BB-640B-4F69-A8C8-D316349120B8}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3680,39 +3680,17 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>54</v>
-      </c>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>

</xml_diff>

<commit_message>
sofia | test3,4,5 | bug fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/test/SSS_Sofia_test4.xlsx
+++ b/assets/fleet/9245263_sofia/test/SSS_Sofia_test4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4CCD52-1671-4FFC-862A-6C4FC33C59D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22553113-D91C-46F5-BBF6-47C8FE0C6F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="59" r:id="rId1"/>
@@ -2625,8 +2625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3047,7 +3047,7 @@
         <v>6.6</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3064,7 +3064,7 @@
         <v>15</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3081,7 +3081,7 @@
         <v>7.8</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3098,7 +3098,7 @@
         <v>10</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -3183,7 +3183,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3200,7 +3200,7 @@
         <v>17</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3217,7 +3217,7 @@
         <v>0</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3234,7 +3234,7 @@
         <v>0.5</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3251,7 +3251,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3268,7 +3268,7 @@
         <v>3</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3302,7 +3302,7 @@
         <v>1.8</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3353,7 +3353,7 @@
         <v>0.4</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3370,7 +3370,7 @@
         <v>6.7</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3387,7 +3387,7 @@
         <v>0.3</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3455,7 +3455,7 @@
         <v>8.4</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3472,7 +3472,7 @@
         <v>6</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3489,7 +3489,7 @@
         <v>6</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3506,7 +3506,7 @@
         <v>3.6</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -3523,7 +3523,7 @@
         <v>3.6</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3638,7 +3638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C7A2BB-640B-4F69-A8C8-D316349120B8}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
sofia | test4 | fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/test/SSS_Sofia_test4.xlsx
+++ b/assets/fleet/9245263_sofia/test/SSS_Sofia_test4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22553113-D91C-46F5-BBF6-47C8FE0C6F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0865A4-C9A6-4825-89B4-358DDE03E89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -691,8 +691,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="0.0"/>
+  <numFmts count="3">
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
@@ -778,7 +777,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
@@ -812,9 +811,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
@@ -858,6 +854,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1226,15 +1231,15 @@
       <c r="A5" t="s">
         <v>193</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>205</v>
       </c>
     </row>
@@ -1267,7 +1272,7 @@
   <cols>
     <col min="2" max="2" width="63" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.25" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.25" style="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.875" customWidth="1"/>
     <col min="6" max="6" width="19.125" customWidth="1"/>
     <col min="9" max="9" width="4.375" bestFit="1" customWidth="1"/>
@@ -1275,34 +1280,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>212</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="24" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
@@ -1314,7 +1319,7 @@
       <c r="C3" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="18">
         <v>7212.7049999999999</v>
       </c>
       <c r="E3" s="10">
@@ -1334,7 +1339,7 @@
       <c r="C4" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="18">
         <v>66.403999999999996</v>
       </c>
       <c r="E4" s="10" t="s">
@@ -1354,7 +1359,7 @@
       <c r="C5" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="18">
         <v>66.403999999999996</v>
       </c>
       <c r="E5" s="10">
@@ -1374,7 +1379,7 @@
       <c r="C6" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="18">
         <v>5.38</v>
       </c>
       <c r="E6" s="10">
@@ -1394,7 +1399,7 @@
       <c r="C7" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="18">
         <v>5.391</v>
       </c>
       <c r="E7" s="10" t="s">
@@ -1414,7 +1419,7 @@
       <c r="C8" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="18">
         <v>0</v>
       </c>
       <c r="E8" s="10" t="s">
@@ -1425,14 +1430,14 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
@@ -1444,7 +1449,7 @@
       <c r="C10" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="18">
         <v>4.3079999999999998</v>
       </c>
       <c r="E10" s="10">
@@ -1464,7 +1469,7 @@
       <c r="C11" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="18">
         <v>4.2</v>
       </c>
       <c r="E11" s="10">
@@ -1484,7 +1489,7 @@
       <c r="C12" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="18">
         <v>4.415</v>
       </c>
       <c r="E12" s="10">
@@ -1504,7 +1509,7 @@
       <c r="C13" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E13" s="10" t="s">
@@ -1524,7 +1529,7 @@
       <c r="C14" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="18">
         <v>-8.0000000000000002E-3</v>
       </c>
       <c r="E14" s="10" t="s">
@@ -1544,7 +1549,7 @@
       <c r="C15" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="18">
         <f>D11-D12</f>
         <v>-0.21499999999999986</v>
       </c>
@@ -1565,7 +1570,7 @@
       <c r="C16" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E16" s="10">
@@ -1585,7 +1590,7 @@
       <c r="C17" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E17" s="10">
@@ -1605,7 +1610,7 @@
       <c r="C18" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E18" s="10">
@@ -1625,7 +1630,7 @@
       <c r="C19" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E19" s="10">
@@ -1645,7 +1650,7 @@
       <c r="C20" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E20" s="10">
@@ -1665,7 +1670,7 @@
       <c r="C21" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E21" s="10">
@@ -1685,7 +1690,7 @@
       <c r="C22" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E22" s="10">
@@ -1705,7 +1710,7 @@
       <c r="C23" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E23" s="10">
@@ -1725,7 +1730,7 @@
       <c r="C24" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E24" s="10">
@@ -1745,7 +1750,7 @@
       <c r="C25" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E25" s="10">
@@ -1765,7 +1770,7 @@
       <c r="C26" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E26" s="10">
@@ -1785,7 +1790,7 @@
       <c r="C27" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E27" s="10">
@@ -1805,7 +1810,7 @@
       <c r="C28" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E28" s="10">
@@ -1825,7 +1830,7 @@
       <c r="C29" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E29" s="10">
@@ -1836,14 +1841,14 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
@@ -1855,7 +1860,7 @@
       <c r="C31" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="D31" s="19">
+      <c r="D31" s="18">
         <v>17.663</v>
       </c>
       <c r="E31" s="10" t="s">
@@ -1875,7 +1880,7 @@
       <c r="C32" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E32" s="10" t="s">
@@ -1895,7 +1900,7 @@
       <c r="C33" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="D33" s="19">
+      <c r="D33" s="18">
         <v>134.86699999999999</v>
       </c>
       <c r="E33" s="10">
@@ -1915,7 +1920,7 @@
       <c r="C34" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D34" s="19" t="s">
+      <c r="D34" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E34" s="10" t="s">
@@ -1935,7 +1940,7 @@
       <c r="C35" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D35" s="19" t="s">
+      <c r="D35" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E35" s="10" t="s">
@@ -1955,7 +1960,7 @@
       <c r="C36" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D36" s="19">
+      <c r="D36" s="18">
         <v>6.8319999999999999</v>
       </c>
       <c r="E36" s="10" t="s">
@@ -1975,7 +1980,7 @@
       <c r="C37" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D37" s="21">
+      <c r="D37" s="20">
         <v>1.4510000000000001</v>
       </c>
       <c r="E37" s="10">
@@ -1995,7 +2000,7 @@
       <c r="C38" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D38" s="21">
+      <c r="D38" s="20">
         <f>68.928/D3</f>
         <v>9.5564701453892814E-3</v>
       </c>
@@ -2017,7 +2022,7 @@
       <c r="C39" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D39" s="21">
+      <c r="D39" s="20">
         <f>6.658/D3</f>
         <v>9.2309334708684195E-4</v>
       </c>
@@ -2038,7 +2043,7 @@
       <c r="C40" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D40" s="19">
+      <c r="D40" s="18">
         <v>1.4410000000000001</v>
       </c>
       <c r="E40" s="10">
@@ -2058,7 +2063,7 @@
       <c r="C41" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D41" s="19" t="s">
+      <c r="D41" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E41" s="10" t="s">
@@ -2078,7 +2083,7 @@
       <c r="C42" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D42" s="19" t="s">
+      <c r="D42" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E42" s="10" t="s">
@@ -2098,7 +2103,7 @@
       <c r="C43" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D43" s="19" t="s">
+      <c r="D43" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E43" s="10">
@@ -2118,7 +2123,7 @@
       <c r="C44" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D44" s="21" t="s">
+      <c r="D44" s="20" t="s">
         <v>54</v>
       </c>
       <c r="E44" s="10" t="s">
@@ -2138,7 +2143,7 @@
       <c r="C45" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D45" s="21" t="s">
+      <c r="D45" s="20" t="s">
         <v>54</v>
       </c>
       <c r="E45" s="10" t="s">
@@ -2158,7 +2163,7 @@
       <c r="C46" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D46" s="19" t="s">
+      <c r="D46" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E46" s="10" t="s">
@@ -2178,7 +2183,7 @@
       <c r="C47" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="D47" s="19" t="s">
+      <c r="D47" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E47" s="10" t="s">
@@ -2198,7 +2203,7 @@
       <c r="C48" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="D48" s="19" t="s">
+      <c r="D48" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E48" s="10" t="s">
@@ -2219,7 +2224,7 @@
       <c r="C49" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D49" s="19" t="s">
+      <c r="D49" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E49" s="10">
@@ -2239,7 +2244,7 @@
       <c r="C50" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D50" s="19">
+      <c r="D50" s="18">
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="E50" s="10">
@@ -2259,7 +2264,7 @@
       <c r="C51" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D51" s="19" t="s">
+      <c r="D51" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E51" s="10">
@@ -2279,7 +2284,7 @@
       <c r="C52" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D52" s="19">
+      <c r="D52" s="18">
         <v>3.75</v>
       </c>
       <c r="E52" s="10" t="s">
@@ -2299,7 +2304,7 @@
       <c r="C53" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D53" s="19" t="s">
+      <c r="D53" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E53" s="10" t="s">
@@ -2319,7 +2324,7 @@
       <c r="C54" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D54" s="19" t="s">
+      <c r="D54" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E54" s="10" t="s">
@@ -2339,7 +2344,7 @@
       <c r="C55" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D55" s="19" t="s">
+      <c r="D55" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E55" s="10" t="s">
@@ -2359,7 +2364,7 @@
       <c r="C56" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="D56" s="19" t="s">
+      <c r="D56" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E56" s="10" t="s">
@@ -2379,7 +2384,7 @@
       <c r="C57" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="D57" s="19" t="s">
+      <c r="D57" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E57" s="10" t="s">
@@ -2399,7 +2404,7 @@
       <c r="C58" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="D58" s="19" t="s">
+      <c r="D58" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E58" s="10" t="s">
@@ -2419,7 +2424,7 @@
       <c r="C59" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D59" s="19" t="s">
+      <c r="D59" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E59" s="10" t="s">
@@ -2439,7 +2444,7 @@
       <c r="C60" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D60" s="19" t="s">
+      <c r="D60" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E60" s="10" t="s">
@@ -2459,7 +2464,7 @@
       <c r="C61" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D61" s="19" t="s">
+      <c r="D61" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E61" s="10" t="s">
@@ -2479,7 +2484,7 @@
       <c r="C62" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="D62" s="19" t="s">
+      <c r="D62" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E62" s="10">
@@ -2499,7 +2504,7 @@
       <c r="C63" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D63" s="19" t="s">
+      <c r="D63" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E63" s="10" t="s">
@@ -2519,7 +2524,7 @@
       <c r="C64" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="D64" s="19" t="s">
+      <c r="D64" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E64" s="10" t="s">
@@ -2539,7 +2544,7 @@
       <c r="C65" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D65" s="19">
+      <c r="D65" s="18">
         <v>0</v>
       </c>
       <c r="E65" s="10" t="s">
@@ -2559,7 +2564,7 @@
       <c r="C66" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D66" s="19">
+      <c r="D66" s="18">
         <v>66.067999999999998</v>
       </c>
       <c r="E66" s="10">
@@ -2579,7 +2584,7 @@
       <c r="C67" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D67" s="19" t="s">
+      <c r="D67" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E67" s="10">
@@ -2599,7 +2604,7 @@
       <c r="C68" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D68" s="24">
+      <c r="D68" s="23">
         <f>D38+D39</f>
         <v>1.0479563492476123E-2</v>
       </c>
@@ -2625,8 +2630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2634,7 +2639,7 @@
     <col min="1" max="1" width="7.75" style="3"/>
     <col min="2" max="2" width="45.125" style="3" customWidth="1"/>
     <col min="3" max="3" width="10.375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="7.75" style="3"/>
+    <col min="4" max="4" width="7.75" style="30"/>
     <col min="5" max="5" width="14.75" style="2" customWidth="1"/>
     <col min="6" max="7" width="7.75" style="2"/>
     <col min="8" max="16384" width="7.75" style="1"/>
@@ -2650,7 +2655,7 @@
       <c r="C1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="28" t="s">
         <v>56</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -2669,7 +2674,7 @@
       <c r="C2" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="29">
         <v>168.91300000000001</v>
       </c>
       <c r="E2" s="11" t="s">
@@ -2686,7 +2691,7 @@
       <c r="C3" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="29">
         <v>135.66499999999999</v>
       </c>
       <c r="E3" s="11" t="s">
@@ -2703,7 +2708,7 @@
       <c r="C4" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="29">
         <v>227.23400000000001</v>
       </c>
       <c r="E4" s="11" t="s">
@@ -2720,7 +2725,7 @@
       <c r="C5" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="29">
         <v>71.417000000000002</v>
       </c>
       <c r="E5" s="11" t="s">
@@ -2737,7 +2742,7 @@
       <c r="C6" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="29">
         <v>240.21899999999999</v>
       </c>
       <c r="E6" s="11" t="s">
@@ -2754,7 +2759,7 @@
       <c r="C7" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="29">
         <v>129.84800000000001</v>
       </c>
       <c r="E7" s="11" t="s">
@@ -2771,7 +2776,7 @@
       <c r="C8" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="29">
         <v>84.581000000000003</v>
       </c>
       <c r="E8" s="11" t="s">
@@ -2788,7 +2793,7 @@
       <c r="C9" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="29">
         <v>84.578999999999994</v>
       </c>
       <c r="E9" s="11" t="s">
@@ -2805,7 +2810,7 @@
       <c r="C10" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="29">
         <v>128.392</v>
       </c>
       <c r="E10" s="11" t="s">
@@ -2822,7 +2827,7 @@
       <c r="C11" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="29">
         <v>128.392</v>
       </c>
       <c r="E11" s="11" t="s">
@@ -2839,7 +2844,7 @@
       <c r="C12" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="29">
         <v>109.261</v>
       </c>
       <c r="E12" s="11" t="s">
@@ -2856,7 +2861,7 @@
       <c r="C13" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="29">
         <v>109.261</v>
       </c>
       <c r="E13" s="11" t="s">
@@ -2873,7 +2878,7 @@
       <c r="C14" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="29">
         <v>129.94499999999999</v>
       </c>
       <c r="E14" s="11" t="s">
@@ -2890,7 +2895,7 @@
       <c r="C15" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="29">
         <v>129.94499999999999</v>
       </c>
       <c r="E15" s="11" t="s">
@@ -2907,7 +2912,7 @@
       <c r="C16" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="29">
         <v>162.61000000000001</v>
       </c>
       <c r="E16" s="11" t="s">
@@ -2924,7 +2929,7 @@
       <c r="C17" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="29">
         <v>162.61000000000001</v>
       </c>
       <c r="E17" s="11" t="s">
@@ -2941,7 +2946,7 @@
       <c r="C18" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="29">
         <v>188.26900000000001</v>
       </c>
       <c r="E18" s="11" t="s">
@@ -2958,7 +2963,7 @@
       <c r="C19" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="29">
         <v>390.197</v>
       </c>
       <c r="E19" s="11" t="s">
@@ -2975,7 +2980,7 @@
       <c r="C20" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="29">
         <v>265.702</v>
       </c>
       <c r="E20" s="11" t="s">
@@ -2992,7 +2997,7 @@
       <c r="C21" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="29">
         <v>265.702</v>
       </c>
       <c r="E21" s="11" t="s">
@@ -3009,7 +3014,7 @@
       <c r="C22" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="29">
         <v>217.238</v>
       </c>
       <c r="E22" s="11" t="s">
@@ -3026,7 +3031,7 @@
       <c r="C23" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="29">
         <v>217.238</v>
       </c>
       <c r="E23" s="11" t="s">
@@ -3043,8 +3048,8 @@
       <c r="C24" s="12">
         <v>0.97</v>
       </c>
-      <c r="D24" s="13">
-        <v>6.6</v>
+      <c r="D24" s="29">
+        <v>6.56</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>191</v>
@@ -3060,7 +3065,7 @@
       <c r="C25" s="12">
         <v>0.97</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D25" s="29">
         <v>15</v>
       </c>
       <c r="E25" s="11" t="s">
@@ -3077,8 +3082,8 @@
       <c r="C26" s="12">
         <v>0.97</v>
       </c>
-      <c r="D26" s="13">
-        <v>7.8</v>
+      <c r="D26" s="29">
+        <v>7.7729999999999997</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>191</v>
@@ -3094,8 +3099,8 @@
       <c r="C27" s="12">
         <v>0.97</v>
       </c>
-      <c r="D27" s="13">
-        <v>10</v>
+      <c r="D27" s="29">
+        <v>9.952</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>191</v>
@@ -3105,13 +3110,13 @@
       <c r="A28" s="3">
         <v>229</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C28" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D28" s="13">
+      <c r="D28" s="29">
         <v>11.227</v>
       </c>
       <c r="E28" s="11" t="s">
@@ -3122,13 +3127,13 @@
       <c r="A29" s="3">
         <v>230</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C29" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D29" s="29">
         <v>11.227</v>
       </c>
       <c r="E29" s="11" t="s">
@@ -3139,13 +3144,13 @@
       <c r="A30" s="3">
         <v>231</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C30" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D30" s="13">
+      <c r="D30" s="29">
         <v>0</v>
       </c>
       <c r="E30" s="11" t="s">
@@ -3156,13 +3161,13 @@
       <c r="A31" s="3">
         <v>232</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C31" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D31" s="13">
+      <c r="D31" s="29">
         <v>0</v>
       </c>
       <c r="E31" s="11" t="s">
@@ -3170,34 +3175,34 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="15">
+      <c r="A32" s="14">
         <v>301</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="13" t="s">
         <v>52</v>
       </c>
       <c r="C32" s="12">
         <v>0.97</v>
       </c>
-      <c r="D32" s="13">
-        <v>2</v>
+      <c r="D32" s="29">
+        <v>1.9670000000000001</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="15">
+      <c r="A33" s="14">
         <v>302</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="13" t="s">
         <v>29</v>
       </c>
       <c r="C33" s="12">
         <v>0.97</v>
       </c>
-      <c r="D33" s="13">
-        <v>17</v>
+      <c r="D33" s="29">
+        <v>17.032</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>191</v>
@@ -3213,7 +3218,7 @@
       <c r="C34" s="12">
         <v>0.97</v>
       </c>
-      <c r="D34" s="13">
+      <c r="D34" s="29">
         <v>0</v>
       </c>
       <c r="E34" s="11" t="s">
@@ -3230,8 +3235,8 @@
       <c r="C35" s="12">
         <v>0.85</v>
       </c>
-      <c r="D35" s="13">
-        <v>0.5</v>
+      <c r="D35" s="29">
+        <v>0.51900000000000002</v>
       </c>
       <c r="E35" s="11" t="s">
         <v>191</v>
@@ -3247,8 +3252,8 @@
       <c r="C36" s="12">
         <v>0.85</v>
       </c>
-      <c r="D36" s="13">
-        <v>4.4000000000000004</v>
+      <c r="D36" s="29">
+        <v>4.4109999999999996</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>191</v>
@@ -3264,8 +3269,8 @@
       <c r="C37" s="12">
         <v>0.85</v>
       </c>
-      <c r="D37" s="13">
-        <v>3</v>
+      <c r="D37" s="29">
+        <v>2.9889999999999999</v>
       </c>
       <c r="E37" s="11" t="s">
         <v>191</v>
@@ -3281,7 +3286,7 @@
       <c r="C38" s="12">
         <v>0.85</v>
       </c>
-      <c r="D38" s="13">
+      <c r="D38" s="29">
         <v>0</v>
       </c>
       <c r="E38" s="11" t="s">
@@ -3298,8 +3303,8 @@
       <c r="C39" s="12">
         <v>0.9</v>
       </c>
-      <c r="D39" s="13">
-        <v>1.8</v>
+      <c r="D39" s="29">
+        <v>1.752</v>
       </c>
       <c r="E39" s="11" t="s">
         <v>191</v>
@@ -3315,7 +3320,7 @@
       <c r="C40" s="12">
         <v>0.9</v>
       </c>
-      <c r="D40" s="13">
+      <c r="D40" s="29">
         <v>0</v>
       </c>
       <c r="E40" s="11" t="s">
@@ -3332,7 +3337,7 @@
       <c r="C41" s="12">
         <v>0.9</v>
       </c>
-      <c r="D41" s="13">
+      <c r="D41" s="29">
         <v>0</v>
       </c>
       <c r="E41" s="11" t="s">
@@ -3349,8 +3354,8 @@
       <c r="C42" s="12">
         <v>0.9</v>
       </c>
-      <c r="D42" s="13">
-        <v>0.4</v>
+      <c r="D42" s="29">
+        <v>0.376</v>
       </c>
       <c r="E42" s="11" t="s">
         <v>191</v>
@@ -3366,8 +3371,8 @@
       <c r="C43" s="12">
         <v>0.97</v>
       </c>
-      <c r="D43" s="13">
-        <v>6.7</v>
+      <c r="D43" s="29">
+        <v>6.6680000000000001</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>191</v>
@@ -3383,8 +3388,8 @@
       <c r="C44" s="12">
         <v>1</v>
       </c>
-      <c r="D44" s="13">
-        <v>0.3</v>
+      <c r="D44" s="29">
+        <v>0.27300000000000002</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>191</v>
@@ -3400,7 +3405,7 @@
       <c r="C45" s="12">
         <v>1</v>
       </c>
-      <c r="D45" s="13">
+      <c r="D45" s="29">
         <v>0</v>
       </c>
       <c r="E45" s="11" t="s">
@@ -3417,7 +3422,7 @@
       <c r="C46" s="12">
         <v>1</v>
       </c>
-      <c r="D46" s="13">
+      <c r="D46" s="29">
         <v>0</v>
       </c>
       <c r="E46" s="11" t="s">
@@ -3434,7 +3439,7 @@
       <c r="C47" s="12">
         <v>1</v>
       </c>
-      <c r="D47" s="13">
+      <c r="D47" s="29">
         <v>0</v>
       </c>
       <c r="E47" s="11" t="s">
@@ -3451,8 +3456,8 @@
       <c r="C48" s="12">
         <v>1</v>
       </c>
-      <c r="D48" s="13">
-        <v>8.4</v>
+      <c r="D48" s="29">
+        <v>8.3740000000000006</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>191</v>
@@ -3468,8 +3473,8 @@
       <c r="C49" s="12">
         <v>1</v>
       </c>
-      <c r="D49" s="13">
-        <v>6</v>
+      <c r="D49" s="29">
+        <v>5.9939999999999998</v>
       </c>
       <c r="E49" s="11" t="s">
         <v>191</v>
@@ -3485,8 +3490,8 @@
       <c r="C50" s="12">
         <v>1</v>
       </c>
-      <c r="D50" s="13">
-        <v>6</v>
+      <c r="D50" s="29">
+        <v>5.9939999999999998</v>
       </c>
       <c r="E50" s="11" t="s">
         <v>191</v>
@@ -3502,8 +3507,8 @@
       <c r="C51" s="12">
         <v>1</v>
       </c>
-      <c r="D51" s="13">
-        <v>3.6</v>
+      <c r="D51" s="29">
+        <v>3.6339999999999999</v>
       </c>
       <c r="E51" s="11" t="s">
         <v>191</v>
@@ -3519,8 +3524,8 @@
       <c r="C52" s="12">
         <v>1</v>
       </c>
-      <c r="D52" s="13">
-        <v>3.6</v>
+      <c r="D52" s="29">
+        <v>3.6339999999999999</v>
       </c>
       <c r="E52" s="11" t="s">
         <v>191</v>
@@ -3536,7 +3541,7 @@
       <c r="C53" s="12">
         <v>0</v>
       </c>
-      <c r="D53" s="13">
+      <c r="D53" s="29">
         <v>0</v>
       </c>
       <c r="E53" s="11" t="s">
@@ -3695,11 +3700,11 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
-      <c r="C3" s="17"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="10"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
@@ -3708,11 +3713,11 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
-      <c r="C4" s="17"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="10"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
@@ -3721,11 +3726,11 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
-      <c r="C5" s="17"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="10"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
@@ -3734,11 +3739,11 @@
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
-      <c r="C6" s="17"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
@@ -3747,11 +3752,11 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="17"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="10"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
@@ -3760,11 +3765,11 @@
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
-      <c r="C8" s="17"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="10"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
@@ -3773,11 +3778,11 @@
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
-      <c r="C9" s="17"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="10"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
@@ -3786,11 +3791,11 @@
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="17"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="10"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
@@ -3799,11 +3804,11 @@
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
-      <c r="C11" s="17"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
@@ -3812,11 +3817,11 @@
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
-      <c r="C12" s="17"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="10"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
@@ -3825,11 +3830,11 @@
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
-      <c r="C13" s="17"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
@@ -3838,11 +3843,11 @@
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="17"/>
+      <c r="C14" s="16"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
@@ -3851,11 +3856,11 @@
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="17"/>
+      <c r="C15" s="16"/>
       <c r="D15" s="10"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
@@ -3864,11 +3869,11 @@
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
-      <c r="C16" s="17"/>
+      <c r="C16" s="16"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
@@ -3877,11 +3882,11 @@
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
-      <c r="C17" s="17"/>
+      <c r="C17" s="16"/>
       <c r="D17" s="10"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
@@ -3890,11 +3895,11 @@
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="17"/>
+      <c r="C18" s="16"/>
       <c r="D18" s="10"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
@@ -3903,11 +3908,11 @@
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
-      <c r="C19" s="17"/>
+      <c r="C19" s="16"/>
       <c r="D19" s="10"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
@@ -3916,11 +3921,11 @@
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
-      <c r="C20" s="17"/>
+      <c r="C20" s="16"/>
       <c r="D20" s="10"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
@@ -3929,11 +3934,11 @@
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
-      <c r="C21" s="17"/>
+      <c r="C21" s="16"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
@@ -3942,11 +3947,11 @@
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
-      <c r="C22" s="17"/>
+      <c r="C22" s="16"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
@@ -3955,11 +3960,11 @@
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
-      <c r="C23" s="17"/>
+      <c r="C23" s="16"/>
       <c r="D23" s="10"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
       <c r="J23" s="10"/>
@@ -3968,11 +3973,11 @@
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
-      <c r="C24" s="17"/>
+      <c r="C24" s="16"/>
       <c r="D24" s="10"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
@@ -3981,11 +3986,11 @@
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
-      <c r="C25" s="17"/>
+      <c r="C25" s="16"/>
       <c r="D25" s="10"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
       <c r="J25" s="10"/>
@@ -3994,11 +3999,11 @@
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
-      <c r="C26" s="17"/>
+      <c r="C26" s="16"/>
       <c r="D26" s="10"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
       <c r="J26" s="10"/>
@@ -4427,22 +4432,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="24" t="s">
         <v>210</v>
       </c>
     </row>
@@ -4628,16 +4633,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="24" t="s">
         <v>210</v>
       </c>
     </row>
@@ -4645,7 +4650,7 @@
       <c r="A2" s="10">
         <v>0</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="23">
         <v>0</v>
       </c>
       <c r="C2" s="10">
@@ -4659,7 +4664,7 @@
       <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="C3" s="10">
@@ -4673,7 +4678,7 @@
       <c r="A4" s="10">
         <v>5</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <v>0.127</v>
       </c>
       <c r="C4" s="10">
@@ -4687,7 +4692,7 @@
       <c r="A5" s="10">
         <v>10</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="23">
         <v>0.26300000000000001</v>
       </c>
       <c r="C5" s="10">
@@ -4701,7 +4706,7 @@
       <c r="A6" s="10">
         <v>12</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="23">
         <v>0.32200000000000001</v>
       </c>
       <c r="C6" s="10">
@@ -4715,7 +4720,7 @@
       <c r="A7" s="10">
         <v>15</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="23">
         <v>0.41599999999999998</v>
       </c>
       <c r="C7" s="10">
@@ -4729,7 +4734,7 @@
       <c r="A8" s="10">
         <v>20</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="23">
         <v>0.59799999999999998</v>
       </c>
       <c r="C8" s="10">
@@ -4743,7 +4748,7 @@
       <c r="A9" s="10">
         <v>25</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="23">
         <v>0.81899999999999995</v>
       </c>
       <c r="C9" s="10">
@@ -4757,7 +4762,7 @@
       <c r="A10" s="10">
         <v>30</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="23">
         <v>1.0669999999999999</v>
       </c>
       <c r="C10" s="10">
@@ -4771,7 +4776,7 @@
       <c r="A11" s="10">
         <v>40</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="23">
         <v>1.488</v>
       </c>
       <c r="C11" s="10">
@@ -4785,7 +4790,7 @@
       <c r="A12" s="10">
         <v>50</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="23">
         <v>1.7370000000000001</v>
       </c>
       <c r="C12" s="10">
@@ -4799,7 +4804,7 @@
       <c r="A13" s="10">
         <v>60</v>
       </c>
-      <c r="B13" s="24">
+      <c r="B13" s="23">
         <v>1.8080000000000001</v>
       </c>
       <c r="C13" s="10">
@@ -4810,7 +4815,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="18"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
     </row>
@@ -4867,22 +4872,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="24" t="s">
         <v>210</v>
       </c>
     </row>
@@ -4896,7 +4901,7 @@
       <c r="C2" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="10" t="s">
@@ -4919,7 +4924,7 @@
       <c r="C3" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="18">
         <v>3.75</v>
       </c>
       <c r="E3" s="10" t="s">
@@ -4942,7 +4947,7 @@
       <c r="C4" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E4" s="10">
@@ -4965,7 +4970,7 @@
       <c r="C5" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E5" s="10">
@@ -4988,7 +4993,7 @@
       <c r="C6" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E6" s="10">
@@ -5011,7 +5016,7 @@
       <c r="C7" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E7" s="10">
@@ -5034,7 +5039,7 @@
       <c r="C8" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E8" s="10">
@@ -5057,7 +5062,7 @@
       <c r="C9" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E9" s="10">
@@ -5080,7 +5085,7 @@
       <c r="C10" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E10" s="10">
@@ -5103,7 +5108,7 @@
       <c r="C11" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="18">
         <v>59.04</v>
       </c>
       <c r="E11" s="10" t="s">
@@ -5126,7 +5131,7 @@
       <c r="C12" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E12" s="10" t="s">
@@ -5149,7 +5154,7 @@
       <c r="C13" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E13" s="10">
@@ -5172,7 +5177,7 @@
       <c r="C14" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E14" s="10" t="s">
@@ -5195,7 +5200,7 @@
       <c r="C15" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E15" s="10" t="s">
@@ -5218,7 +5223,7 @@
       <c r="C16" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E16" s="10" t="s">
@@ -5241,7 +5246,7 @@
       <c r="C17" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E17" s="10">
@@ -5264,7 +5269,7 @@
       <c r="C18" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="18" t="s">
         <v>54</v>
       </c>
       <c r="E18" s="10">

</xml_diff>

<commit_message>
sofia | test4,5,6 | fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/test/SSS_Sofia_test4.xlsx
+++ b/assets/fleet/9245263_sofia/test/SSS_Sofia_test4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0865A4-C9A6-4825-89B4-358DDE03E89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C660168-D286-4813-AA1B-E780927C0161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="59" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="214">
   <si>
     <t>Форпик</t>
   </si>
@@ -692,9 +692,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="#,##0.000"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -798,10 +798,10 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -810,7 +810,7 @@
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
@@ -825,14 +825,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -841,7 +841,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -853,16 +853,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1265,7 +1265,7 @@
   <dimension ref="A1:L68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1300,14 +1300,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="30" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
@@ -1430,14 +1430,14 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
@@ -1841,14 +1841,14 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="30" t="s">
         <v>175</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
@@ -2630,7 +2630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
@@ -2639,7 +2639,7 @@
     <col min="1" max="1" width="7.75" style="3"/>
     <col min="2" max="2" width="45.125" style="3" customWidth="1"/>
     <col min="3" max="3" width="10.375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="7.75" style="30"/>
+    <col min="4" max="4" width="7.75" style="29"/>
     <col min="5" max="5" width="14.75" style="2" customWidth="1"/>
     <col min="6" max="7" width="7.75" style="2"/>
     <col min="8" max="16384" width="7.75" style="1"/>
@@ -2655,7 +2655,7 @@
       <c r="C1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="27" t="s">
         <v>56</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -2674,7 +2674,7 @@
       <c r="C2" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D2" s="29">
+      <c r="D2" s="28">
         <v>168.91300000000001</v>
       </c>
       <c r="E2" s="11" t="s">
@@ -2691,7 +2691,7 @@
       <c r="C3" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="28">
         <v>135.66499999999999</v>
       </c>
       <c r="E3" s="11" t="s">
@@ -2708,7 +2708,7 @@
       <c r="C4" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="28">
         <v>227.23400000000001</v>
       </c>
       <c r="E4" s="11" t="s">
@@ -2725,7 +2725,7 @@
       <c r="C5" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="28">
         <v>71.417000000000002</v>
       </c>
       <c r="E5" s="11" t="s">
@@ -2742,7 +2742,7 @@
       <c r="C6" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="28">
         <v>240.21899999999999</v>
       </c>
       <c r="E6" s="11" t="s">
@@ -2759,7 +2759,7 @@
       <c r="C7" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="28">
         <v>129.84800000000001</v>
       </c>
       <c r="E7" s="11" t="s">
@@ -2776,7 +2776,7 @@
       <c r="C8" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="28">
         <v>84.581000000000003</v>
       </c>
       <c r="E8" s="11" t="s">
@@ -2793,7 +2793,7 @@
       <c r="C9" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="28">
         <v>84.578999999999994</v>
       </c>
       <c r="E9" s="11" t="s">
@@ -2810,7 +2810,7 @@
       <c r="C10" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="28">
         <v>128.392</v>
       </c>
       <c r="E10" s="11" t="s">
@@ -2827,7 +2827,7 @@
       <c r="C11" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="28">
         <v>128.392</v>
       </c>
       <c r="E11" s="11" t="s">
@@ -2844,7 +2844,7 @@
       <c r="C12" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D12" s="28">
         <v>109.261</v>
       </c>
       <c r="E12" s="11" t="s">
@@ -2861,7 +2861,7 @@
       <c r="C13" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="28">
         <v>109.261</v>
       </c>
       <c r="E13" s="11" t="s">
@@ -2878,7 +2878,7 @@
       <c r="C14" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="28">
         <v>129.94499999999999</v>
       </c>
       <c r="E14" s="11" t="s">
@@ -2895,7 +2895,7 @@
       <c r="C15" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="28">
         <v>129.94499999999999</v>
       </c>
       <c r="E15" s="11" t="s">
@@ -2912,7 +2912,7 @@
       <c r="C16" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D16" s="28">
         <v>162.61000000000001</v>
       </c>
       <c r="E16" s="11" t="s">
@@ -2929,7 +2929,7 @@
       <c r="C17" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D17" s="28">
         <v>162.61000000000001</v>
       </c>
       <c r="E17" s="11" t="s">
@@ -2946,7 +2946,7 @@
       <c r="C18" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D18" s="29">
+      <c r="D18" s="28">
         <v>188.26900000000001</v>
       </c>
       <c r="E18" s="11" t="s">
@@ -2963,7 +2963,7 @@
       <c r="C19" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D19" s="29">
+      <c r="D19" s="28">
         <v>390.197</v>
       </c>
       <c r="E19" s="11" t="s">
@@ -2980,7 +2980,7 @@
       <c r="C20" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D20" s="29">
+      <c r="D20" s="28">
         <v>265.702</v>
       </c>
       <c r="E20" s="11" t="s">
@@ -2997,7 +2997,7 @@
       <c r="C21" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D21" s="29">
+      <c r="D21" s="28">
         <v>265.702</v>
       </c>
       <c r="E21" s="11" t="s">
@@ -3014,7 +3014,7 @@
       <c r="C22" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D22" s="29">
+      <c r="D22" s="28">
         <v>217.238</v>
       </c>
       <c r="E22" s="11" t="s">
@@ -3031,7 +3031,7 @@
       <c r="C23" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D23" s="29">
+      <c r="D23" s="28">
         <v>217.238</v>
       </c>
       <c r="E23" s="11" t="s">
@@ -3048,7 +3048,7 @@
       <c r="C24" s="12">
         <v>0.97</v>
       </c>
-      <c r="D24" s="29">
+      <c r="D24" s="28">
         <v>6.56</v>
       </c>
       <c r="E24" s="11" t="s">
@@ -3065,7 +3065,7 @@
       <c r="C25" s="12">
         <v>0.97</v>
       </c>
-      <c r="D25" s="29">
+      <c r="D25" s="28">
         <v>15</v>
       </c>
       <c r="E25" s="11" t="s">
@@ -3082,7 +3082,7 @@
       <c r="C26" s="12">
         <v>0.97</v>
       </c>
-      <c r="D26" s="29">
+      <c r="D26" s="28">
         <v>7.7729999999999997</v>
       </c>
       <c r="E26" s="11" t="s">
@@ -3099,7 +3099,7 @@
       <c r="C27" s="12">
         <v>0.97</v>
       </c>
-      <c r="D27" s="29">
+      <c r="D27" s="28">
         <v>9.952</v>
       </c>
       <c r="E27" s="11" t="s">
@@ -3116,7 +3116,7 @@
       <c r="C28" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D28" s="29">
+      <c r="D28" s="28">
         <v>11.227</v>
       </c>
       <c r="E28" s="11" t="s">
@@ -3133,7 +3133,7 @@
       <c r="C29" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D29" s="29">
+      <c r="D29" s="28">
         <v>11.227</v>
       </c>
       <c r="E29" s="11" t="s">
@@ -3150,7 +3150,7 @@
       <c r="C30" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D30" s="29">
+      <c r="D30" s="28">
         <v>0</v>
       </c>
       <c r="E30" s="11" t="s">
@@ -3167,7 +3167,7 @@
       <c r="C31" s="12">
         <v>1.0249999999999999</v>
       </c>
-      <c r="D31" s="29">
+      <c r="D31" s="28">
         <v>0</v>
       </c>
       <c r="E31" s="11" t="s">
@@ -3184,7 +3184,7 @@
       <c r="C32" s="12">
         <v>0.97</v>
       </c>
-      <c r="D32" s="29">
+      <c r="D32" s="28">
         <v>1.9670000000000001</v>
       </c>
       <c r="E32" s="11" t="s">
@@ -3201,7 +3201,7 @@
       <c r="C33" s="12">
         <v>0.97</v>
       </c>
-      <c r="D33" s="29">
+      <c r="D33" s="28">
         <v>17.032</v>
       </c>
       <c r="E33" s="11" t="s">
@@ -3218,7 +3218,7 @@
       <c r="C34" s="12">
         <v>0.97</v>
       </c>
-      <c r="D34" s="29">
+      <c r="D34" s="28">
         <v>0</v>
       </c>
       <c r="E34" s="11" t="s">
@@ -3235,7 +3235,7 @@
       <c r="C35" s="12">
         <v>0.85</v>
       </c>
-      <c r="D35" s="29">
+      <c r="D35" s="28">
         <v>0.51900000000000002</v>
       </c>
       <c r="E35" s="11" t="s">
@@ -3252,7 +3252,7 @@
       <c r="C36" s="12">
         <v>0.85</v>
       </c>
-      <c r="D36" s="29">
+      <c r="D36" s="28">
         <v>4.4109999999999996</v>
       </c>
       <c r="E36" s="11" t="s">
@@ -3269,7 +3269,7 @@
       <c r="C37" s="12">
         <v>0.85</v>
       </c>
-      <c r="D37" s="29">
+      <c r="D37" s="28">
         <v>2.9889999999999999</v>
       </c>
       <c r="E37" s="11" t="s">
@@ -3286,7 +3286,7 @@
       <c r="C38" s="12">
         <v>0.85</v>
       </c>
-      <c r="D38" s="29">
+      <c r="D38" s="28">
         <v>0</v>
       </c>
       <c r="E38" s="11" t="s">
@@ -3303,7 +3303,7 @@
       <c r="C39" s="12">
         <v>0.9</v>
       </c>
-      <c r="D39" s="29">
+      <c r="D39" s="28">
         <v>1.752</v>
       </c>
       <c r="E39" s="11" t="s">
@@ -3320,7 +3320,7 @@
       <c r="C40" s="12">
         <v>0.9</v>
       </c>
-      <c r="D40" s="29">
+      <c r="D40" s="28">
         <v>0</v>
       </c>
       <c r="E40" s="11" t="s">
@@ -3337,7 +3337,7 @@
       <c r="C41" s="12">
         <v>0.9</v>
       </c>
-      <c r="D41" s="29">
+      <c r="D41" s="28">
         <v>0</v>
       </c>
       <c r="E41" s="11" t="s">
@@ -3354,7 +3354,7 @@
       <c r="C42" s="12">
         <v>0.9</v>
       </c>
-      <c r="D42" s="29">
+      <c r="D42" s="28">
         <v>0.376</v>
       </c>
       <c r="E42" s="11" t="s">
@@ -3371,7 +3371,7 @@
       <c r="C43" s="12">
         <v>0.97</v>
       </c>
-      <c r="D43" s="29">
+      <c r="D43" s="28">
         <v>6.6680000000000001</v>
       </c>
       <c r="E43" s="11" t="s">
@@ -3388,7 +3388,7 @@
       <c r="C44" s="12">
         <v>1</v>
       </c>
-      <c r="D44" s="29">
+      <c r="D44" s="28">
         <v>0.27300000000000002</v>
       </c>
       <c r="E44" s="11" t="s">
@@ -3405,7 +3405,7 @@
       <c r="C45" s="12">
         <v>1</v>
       </c>
-      <c r="D45" s="29">
+      <c r="D45" s="28">
         <v>0</v>
       </c>
       <c r="E45" s="11" t="s">
@@ -3422,7 +3422,7 @@
       <c r="C46" s="12">
         <v>1</v>
       </c>
-      <c r="D46" s="29">
+      <c r="D46" s="28">
         <v>0</v>
       </c>
       <c r="E46" s="11" t="s">
@@ -3439,7 +3439,7 @@
       <c r="C47" s="12">
         <v>1</v>
       </c>
-      <c r="D47" s="29">
+      <c r="D47" s="28">
         <v>0</v>
       </c>
       <c r="E47" s="11" t="s">
@@ -3456,7 +3456,7 @@
       <c r="C48" s="12">
         <v>1</v>
       </c>
-      <c r="D48" s="29">
+      <c r="D48" s="28">
         <v>8.3740000000000006</v>
       </c>
       <c r="E48" s="11" t="s">
@@ -3473,7 +3473,7 @@
       <c r="C49" s="12">
         <v>1</v>
       </c>
-      <c r="D49" s="29">
+      <c r="D49" s="28">
         <v>5.9939999999999998</v>
       </c>
       <c r="E49" s="11" t="s">
@@ -3490,7 +3490,7 @@
       <c r="C50" s="12">
         <v>1</v>
       </c>
-      <c r="D50" s="29">
+      <c r="D50" s="28">
         <v>5.9939999999999998</v>
       </c>
       <c r="E50" s="11" t="s">
@@ -3507,7 +3507,7 @@
       <c r="C51" s="12">
         <v>1</v>
       </c>
-      <c r="D51" s="29">
+      <c r="D51" s="28">
         <v>3.6339999999999999</v>
       </c>
       <c r="E51" s="11" t="s">
@@ -3524,7 +3524,7 @@
       <c r="C52" s="12">
         <v>1</v>
       </c>
-      <c r="D52" s="29">
+      <c r="D52" s="28">
         <v>3.6339999999999999</v>
       </c>
       <c r="E52" s="11" t="s">
@@ -3541,7 +3541,7 @@
       <c r="C53" s="12">
         <v>0</v>
       </c>
-      <c r="D53" s="29">
+      <c r="D53" s="28">
         <v>0</v>
       </c>
       <c r="E53" s="11" t="s">
@@ -4857,8 +4857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E500720D-7F16-4373-97E5-9F957C7E1B58}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5269,8 +5269,8 @@
       <c r="C18" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>54</v>
+      <c r="D18" s="18">
+        <v>1.2</v>
       </c>
       <c r="E18" s="10">
         <v>1</v>

</xml_diff>